<commit_message>
adding the spreadsheet used for finding the most common features
</commit_message>
<xml_diff>
--- a/stage 2 - features selection/reports testing/processing testing results.xlsx
+++ b/stage 2 - features selection/reports testing/processing testing results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="120" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0000000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000000%"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -161,7 +161,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -185,14 +185,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -210,17 +215,20 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="22" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="22" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -231,6 +239,14 @@
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -574,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -584,45 +600,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="29" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="6">
-        <v>1</v>
-      </c>
-      <c r="B3" s="6">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
         <v>0.86670000000000003</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>0.86670000000000003</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>0.93330000000000002</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>0.8</v>
       </c>
     </row>
@@ -635,26 +651,26 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1"/>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="10">
         <f>MEDIAN(A3:E3)</f>
         <v>0.86670000000000003</v>
       </c>
-      <c r="D5" s="9"/>
+      <c r="D5" s="10"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1"/>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <f>STDEV(A3:E3)/SQRT(COUNT(A3:E3))</f>
         <v>3.3988889361083859E-2</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="9"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:7">
@@ -665,45 +681,45 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="29" customHeight="1">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>0.8</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>0.93330000000000002</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>0.93330000000000002</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>0.93330000000000002</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>0.8</v>
       </c>
     </row>
@@ -716,28 +732,28 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1"/>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="10">
         <f>AVERAGE(A10:E10)</f>
         <v>0.87997999999999998</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1"/>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <f>STDEV(A10:E10)/SQRT(COUNT(A10:E10))</f>
         <v>3.265169827129976E-2</v>
       </c>
-      <c r="D13" s="10"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:7">
@@ -748,45 +764,45 @@
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="29" customHeight="1">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="11" t="s">
+      <c r="A16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="6">
-        <v>1</v>
-      </c>
-      <c r="B17" s="6">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6">
-        <v>1</v>
-      </c>
-      <c r="D17" s="6">
-        <v>1</v>
-      </c>
-      <c r="E17" s="6">
+      <c r="A17" s="5">
+        <v>1</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5">
         <v>1</v>
       </c>
     </row>
@@ -799,28 +815,28 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1"/>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="10">
         <f>MEDIAN(A17:E17)</f>
         <v>1</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1"/>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <f>STDEV(A17:E17)/SQRT(COUNT(A17:E17))</f>
         <v>0</v>
       </c>
-      <c r="D20" s="10"/>
+      <c r="D20" s="9"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:7">
@@ -831,45 +847,45 @@
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:7" ht="29" customHeight="1">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="11" t="s">
+      <c r="A23" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="6">
+      <c r="A24" s="5">
         <v>0.86670000000000003</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>0.86670000000000003</v>
       </c>
-      <c r="C24" s="6">
-        <v>1</v>
-      </c>
-      <c r="D24" s="6">
+      <c r="C24" s="5">
+        <v>1</v>
+      </c>
+      <c r="D24" s="5">
         <v>0.8</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="5">
         <v>0.8</v>
       </c>
     </row>
@@ -882,28 +898,28 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="1"/>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="10">
         <f>AVERAGE(A24:E24)</f>
         <v>0.86668000000000001</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="1"/>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="9">
         <f>STDEV(A24:E24)/SQRT(COUNT(A24:E24))</f>
         <v>3.6514838079881977E-2</v>
       </c>
-      <c r="D27" s="10"/>
+      <c r="D27" s="9"/>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:7">
@@ -914,45 +930,45 @@
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:7" ht="29" customHeight="1">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="11" t="s">
+      <c r="A30" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="6">
+      <c r="A31" s="5">
         <v>0.86670000000000003</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <v>0.86670000000000003</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="5">
         <v>0.93330000000000002</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <v>0.8</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <v>0.8</v>
       </c>
     </row>
@@ -965,37 +981,32 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="1"/>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="10">
         <f>AVERAGE(A31:E31)</f>
         <v>0.85333999999999999</v>
       </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="1"/>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="9">
         <f>STDEV(A31:E31)/SQRT(COUNT(A31:E31))</f>
         <v>2.4940821959189712E-2</v>
       </c>
-      <c r="D34" s="10"/>
+      <c r="D34" s="9"/>
       <c r="E34" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="A15:E15"/>
@@ -1006,6 +1017,11 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A30" r:id="rId1"/>

</xml_diff>